<commit_message>
Report 8_15 Ready to launch :wink::smiley:
</commit_message>
<xml_diff>
--- a/Dates.xlsx
+++ b/Dates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3862DD90-8A1B-48F3-961C-CD7559070BC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C71596-3413-47D6-A51F-3E9AE613F277}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -152,15 +152,21 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,7 +455,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,11 +466,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -478,11 +484,11 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">

</xml_diff>

<commit_message>
Playing with Excel :grin:
</commit_message>
<xml_diff>
--- a/Dates.xlsx
+++ b/Dates.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL-SP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C71596-3413-47D6-A51F-3E9AE613F277}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D76623-C3E5-4699-A1D5-BB076A35A745}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="فروردین" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -152,12 +152,6 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -166,6 +160,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,29 +466,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">

</xml_diff>